<commit_message>
reverted from gp#m# naming scheme because that did not work
</commit_message>
<xml_diff>
--- a/WT_Levelwalk_DLC_for_AutoGaitA/WT_Levelwalk_DLC_Annotation_Table_brief.xlsx
+++ b/WT_Levelwalk_DLC_for_AutoGaitA/WT_Levelwalk_DLC_Annotation_Table_brief.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="8">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">Stance (te)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gp3m3</t>
   </si>
   <si>
     <t xml:space="preserve">levelwalk</t>
@@ -304,7 +301,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.15"/>
@@ -930,11 +927,11 @@
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="4" t="n">
+        <v>303</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>1</v>
@@ -1186,7 +1183,7 @@
         <v>501</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1414,7 +1411,7 @@
         <v>503</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1525,7 +1522,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2</v>

</xml_diff>